<commit_message>
Made R script that creates boxplot of genome sizes
</commit_message>
<xml_diff>
--- a/STEP2/Contigs.xlsx
+++ b/STEP2/Contigs.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
-    <t xml:space="preserve">Organisms</t>
+    <t xml:space="preserve">Species</t>
   </si>
   <si>
     <t xml:space="preserve">Contigs</t>
@@ -731,15 +731,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -750,11 +741,11 @@
   </sheetPr>
   <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -767,12 +758,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.46"/>
@@ -798,20 +789,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="16.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="26.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="12.83"/>
@@ -829,8 +820,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="8.94"/>
@@ -848,7 +839,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="25.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="24.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="25.47"/>
@@ -877,16 +868,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="0" width="34.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="0" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="129" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="130" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="131" min="131" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="132" min="132" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="136" min="136" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="137" style="0" width="12.83"/>
@@ -928,7 +919,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="173" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="174" style="0" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="175" min="175" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="176" min="176" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="176" min="176" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="177" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="179" min="179" style="0" width="17.55"/>

</xml_diff>